<commit_message>
AF-611 tests for named ranges and area intersections are moved to temporary_excel_files
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Error_Name.xlsx
+++ b/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Error_Name.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\SpreadSheet\master\calculation-engine\engine-core-demo\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-tests\engine-it-graph\src\test\resources\standard_excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -362,9 +362,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="e">
-        <f>CONCATENATE(text,A2)</f>
-        <v>#NAME?</v>
+      <c r="B2" s="1" t="str">
+        <f>CONCATENATE(A1,A2)</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -373,12 +373,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -496,19 +493,43 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB3CA02-842D-4858-B4DC-815791FF2F3F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F2BA20-BECB-4812-B9C6-3439A4D658F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CAD8467-C25B-4F00-AE5B-358CD49E6E84}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CAD8467-C25B-4F00-AE5B-358CD49E6E84}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F2BA20-BECB-4812-B9C6-3439A4D658F3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB3CA02-842D-4858-B4DC-815791FF2F3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
#129 adding support of named ranges for DataModel class
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Error_Name.xlsx
+++ b/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Error_Name.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-tests\engine-it-graph\src\test\resources\standard_excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\SpreadSheet\master\calculation-engine\engine-core-demo\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -362,9 +362,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="str">
-        <f>CONCATENATE(A1,A2)</f>
-        <v/>
+      <c r="B2" s="1" t="e">
+        <f>CONCATENATE(text,A2)</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -373,9 +373,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -493,43 +496,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F2BA20-BECB-4812-B9C6-3439A4D658F3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB3CA02-842D-4858-B4DC-815791FF2F3F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CAD8467-C25B-4F00-AE5B-358CD49E6E84}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CAD8467-C25B-4F00-AE5B-358CD49E6E84}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB3CA02-842D-4858-B4DC-815791FF2F3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F2BA20-BECB-4812-B9C6-3439A4D658F3}"/>
 </file>
</xml_diff>